<commit_message>
all plants were added
</commit_message>
<xml_diff>
--- a/references/20240423_data-mapping-mat20.xlsx
+++ b/references/20240423_data-mapping-mat20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sepujas\Dev\mat2\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sepujas\Dev\mat\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5DB35D-0F46-48C1-87CB-57AA453DE804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E39C59-F7FA-4C83-809C-79AD6A9F1674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{AB58512C-90A7-4B4B-B2B2-3EFAE313B693}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12735" activeTab="1" xr2:uid="{AB58512C-90A7-4B4B-B2B2-3EFAE313B693}"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_SCM_materials" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="611">
   <si>
     <t>Plant</t>
   </si>
@@ -1869,6 +1869,15 @@
   </si>
   <si>
     <t>vba_material_mocl.vbs</t>
+  </si>
+  <si>
+    <t>C:\Users\sepujas\Dev\mat\references\vba</t>
+  </si>
+  <si>
+    <t>c:\Users\sepujas\Dev\mat\data\raw</t>
+  </si>
+  <si>
+    <t>C:\Users\sepujas\Dev\mat\references\vba\tbl_stock_mb52.txt</t>
   </si>
 </sst>
 </file>
@@ -3515,34 +3524,34 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AJ36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" customWidth="1"/>
-    <col min="3" max="6" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.08984375" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" customWidth="1"/>
-    <col min="16" max="16" width="10.90625" customWidth="1"/>
-    <col min="18" max="18" width="16.26953125" customWidth="1"/>
-    <col min="20" max="20" width="10.90625" customWidth="1"/>
-    <col min="21" max="21" width="10.453125" customWidth="1"/>
-    <col min="22" max="22" width="11.453125" customWidth="1"/>
-    <col min="28" max="28" width="15.453125" customWidth="1"/>
-    <col min="29" max="29" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" customWidth="1"/>
     <col min="30" max="30" width="10" customWidth="1"/>
-    <col min="31" max="31" width="0.90625" customWidth="1"/>
-    <col min="32" max="32" width="18.26953125" customWidth="1"/>
-    <col min="33" max="33" width="18.08984375" customWidth="1"/>
+    <col min="31" max="31" width="0.85546875" customWidth="1"/>
+    <col min="32" max="32" width="18.28515625" customWidth="1"/>
+    <col min="33" max="33" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -3559,7 +3568,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -3576,7 +3585,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -3593,7 +3602,7 @@
         <v>8330</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>88</v>
       </c>
@@ -3610,7 +3619,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>90</v>
       </c>
@@ -3627,7 +3636,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>238</v>
       </c>
@@ -3644,7 +3653,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>235</v>
       </c>
@@ -3661,7 +3670,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="AF9" t="s">
         <v>98</v>
       </c>
@@ -3669,7 +3678,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -3767,7 +3776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -3865,7 +3874,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -3963,49 +3972,49 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="AF15" s="17"/>
       <c r="AG15" s="18"/>
       <c r="AH15" s="18"/>
       <c r="AI15" s="18"/>
       <c r="AJ15" s="19"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="AF16" s="20"/>
       <c r="AG16" s="21"/>
       <c r="AH16" s="21"/>
       <c r="AI16" s="21"/>
       <c r="AJ16" s="22"/>
     </row>
-    <row r="17" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:36" x14ac:dyDescent="0.2">
       <c r="AF17" s="20"/>
       <c r="AG17" s="21"/>
       <c r="AH17" s="21"/>
       <c r="AI17" s="21"/>
       <c r="AJ17" s="22"/>
     </row>
-    <row r="18" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:36" x14ac:dyDescent="0.2">
       <c r="AF18" s="20"/>
       <c r="AG18" s="21"/>
       <c r="AH18" s="21"/>
       <c r="AI18" s="21"/>
       <c r="AJ18" s="22"/>
     </row>
-    <row r="19" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:36" x14ac:dyDescent="0.2">
       <c r="AF19" s="20"/>
       <c r="AG19" s="21"/>
       <c r="AH19" s="21"/>
       <c r="AI19" s="21"/>
       <c r="AJ19" s="22"/>
     </row>
-    <row r="20" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:36" x14ac:dyDescent="0.2">
       <c r="AF20" s="20"/>
       <c r="AG20" s="21"/>
       <c r="AH20" s="21"/>
       <c r="AI20" s="21"/>
       <c r="AJ20" s="22"/>
     </row>
-    <row r="21" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H21">
         <v>8650</v>
       </c>
@@ -4018,7 +4027,7 @@
       <c r="AI21" s="21"/>
       <c r="AJ21" s="22"/>
     </row>
-    <row r="22" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H22">
         <v>8750</v>
       </c>
@@ -4031,7 +4040,7 @@
       <c r="AI22" s="21"/>
       <c r="AJ22" s="22"/>
     </row>
-    <row r="23" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H23">
         <v>3000</v>
       </c>
@@ -4044,7 +4053,7 @@
       <c r="AI23" s="21"/>
       <c r="AJ23" s="22"/>
     </row>
-    <row r="24" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H24">
         <v>8300</v>
       </c>
@@ -4057,7 +4066,7 @@
       <c r="AI24" s="21"/>
       <c r="AJ24" s="22"/>
     </row>
-    <row r="25" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:36" x14ac:dyDescent="0.2">
       <c r="J25" t="s">
         <v>604</v>
       </c>
@@ -4067,7 +4076,7 @@
       <c r="AI25" s="21"/>
       <c r="AJ25" s="22"/>
     </row>
-    <row r="26" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H26">
         <v>8650</v>
       </c>
@@ -4077,7 +4086,7 @@
       <c r="AI26" s="21"/>
       <c r="AJ26" s="22"/>
     </row>
-    <row r="27" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H27">
         <v>8750</v>
       </c>
@@ -4090,7 +4099,7 @@
       <c r="AI27" s="21"/>
       <c r="AJ27" s="22"/>
     </row>
-    <row r="28" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H28">
         <v>3000</v>
       </c>
@@ -4103,7 +4112,7 @@
       <c r="AI28" s="24"/>
       <c r="AJ28" s="25"/>
     </row>
-    <row r="29" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H29">
         <v>8330</v>
       </c>
@@ -4111,17 +4120,17 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="30" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:36" x14ac:dyDescent="0.2">
       <c r="J30">
         <v>8330</v>
       </c>
     </row>
-    <row r="31" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:36" x14ac:dyDescent="0.2">
       <c r="J31" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="8:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:36" x14ac:dyDescent="0.2">
       <c r="H32" t="s">
         <v>592</v>
       </c>
@@ -4129,7 +4138,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H33" t="s">
         <v>596</v>
       </c>
@@ -4137,7 +4146,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H34" t="s">
         <v>597</v>
       </c>
@@ -4145,7 +4154,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="35" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H35" t="s">
         <v>598</v>
       </c>
@@ -4153,7 +4162,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="36" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H36" t="s">
         <v>599</v>
       </c>
@@ -4188,9 +4197,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>130</v>
       </c>
@@ -4198,7 +4207,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>456</v>
       </c>
@@ -4206,7 +4215,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>458</v>
       </c>
@@ -4214,7 +4223,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>460</v>
       </c>
@@ -4222,7 +4231,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>462</v>
       </c>
@@ -4230,7 +4239,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>464</v>
       </c>
@@ -4238,7 +4247,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>466</v>
       </c>
@@ -4246,7 +4255,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>468</v>
       </c>
@@ -4254,7 +4263,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>470</v>
       </c>
@@ -4262,7 +4271,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>472</v>
       </c>
@@ -4270,7 +4279,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>474</v>
       </c>
@@ -4278,7 +4287,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>476</v>
       </c>
@@ -4286,7 +4295,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>478</v>
       </c>
@@ -4294,7 +4303,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>480</v>
       </c>
@@ -4302,7 +4311,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>482</v>
       </c>
@@ -4310,7 +4319,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>484</v>
       </c>
@@ -4318,7 +4327,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>486</v>
       </c>
@@ -4326,7 +4335,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>488</v>
       </c>
@@ -4334,7 +4343,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>490</v>
       </c>
@@ -4342,7 +4351,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>492</v>
       </c>
@@ -4350,7 +4359,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>494</v>
       </c>
@@ -4358,7 +4367,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>496</v>
       </c>
@@ -4366,7 +4375,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>498</v>
       </c>
@@ -4374,7 +4383,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>500</v>
       </c>
@@ -4382,7 +4391,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>502</v>
       </c>
@@ -4390,7 +4399,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>504</v>
       </c>
@@ -4398,7 +4407,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>506</v>
       </c>
@@ -4406,7 +4415,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>508</v>
       </c>
@@ -4414,7 +4423,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>510</v>
       </c>
@@ -4422,7 +4431,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>512</v>
       </c>
@@ -4430,7 +4439,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>514</v>
       </c>
@@ -4438,7 +4447,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>516</v>
       </c>
@@ -4446,7 +4455,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>518</v>
       </c>
@@ -4454,7 +4463,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>520</v>
       </c>
@@ -4462,7 +4471,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>522</v>
       </c>
@@ -4470,7 +4479,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>524</v>
       </c>
@@ -4478,7 +4487,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>526</v>
       </c>
@@ -4486,7 +4495,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>528</v>
       </c>
@@ -4494,7 +4503,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>530</v>
       </c>
@@ -4502,7 +4511,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>532</v>
       </c>
@@ -4510,7 +4519,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>534</v>
       </c>
@@ -4518,7 +4527,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>536</v>
       </c>
@@ -4526,7 +4535,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>538</v>
       </c>
@@ -4534,7 +4543,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>540</v>
       </c>
@@ -4542,7 +4551,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>542</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>544</v>
       </c>
@@ -4558,7 +4567,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>546</v>
       </c>
@@ -4566,7 +4575,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>548</v>
       </c>
@@ -4574,7 +4583,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>549</v>
       </c>
@@ -4582,7 +4591,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>550</v>
       </c>
@@ -4590,7 +4599,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>552</v>
       </c>
@@ -4598,7 +4607,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>554</v>
       </c>
@@ -4606,7 +4615,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>556</v>
       </c>
@@ -4614,7 +4623,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>558</v>
       </c>
@@ -4637,34 +4646,34 @@
   </sheetPr>
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" customWidth="1"/>
-    <col min="13" max="13" width="14.36328125" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="0.90625" customWidth="1"/>
-    <col min="16" max="16" width="18.26953125" customWidth="1"/>
-    <col min="17" max="17" width="18.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="0.85546875" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -4682,7 +4691,7 @@
       </c>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -4700,7 +4709,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -4718,7 +4727,7 @@
       </c>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>88</v>
       </c>
@@ -4736,7 +4745,7 @@
       </c>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>90</v>
       </c>
@@ -4754,16 +4763,16 @@
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>91</v>
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P9" t="s">
         <v>98</v>
       </c>
@@ -4771,7 +4780,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -4821,7 +4830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -4871,7 +4880,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -4921,7 +4930,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P15" s="26"/>
       <c r="Q15" s="26"/>
       <c r="R15" s="26"/>
@@ -4929,7 +4938,7 @@
       <c r="T15" s="26"/>
       <c r="U15" s="26"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26"/>
@@ -4937,7 +4946,10 @@
       <c r="T16" s="26"/>
       <c r="U16" s="26"/>
     </row>
-    <row r="17" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>610</v>
+      </c>
       <c r="P17" s="26"/>
       <c r="Q17" s="26"/>
       <c r="R17" s="26"/>
@@ -4945,7 +4957,10 @@
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
     </row>
-    <row r="18" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>608</v>
+      </c>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
       <c r="R18" s="26"/>
@@ -4953,7 +4968,10 @@
       <c r="T18" s="26"/>
       <c r="U18" s="26"/>
     </row>
-    <row r="19" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>609</v>
+      </c>
       <c r="P19" s="26"/>
       <c r="Q19" s="26"/>
       <c r="R19" s="26"/>
@@ -4961,7 +4979,10 @@
       <c r="T19" s="26"/>
       <c r="U19" s="26"/>
     </row>
-    <row r="20" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>586</v>
+      </c>
       <c r="P20" s="26"/>
       <c r="Q20" s="26"/>
       <c r="R20" s="26"/>
@@ -4969,7 +4990,10 @@
       <c r="T20" s="26"/>
       <c r="U20" s="26"/>
     </row>
-    <row r="21" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>587</v>
+      </c>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
@@ -4977,7 +5001,7 @@
       <c r="T21" s="26"/>
       <c r="U21" s="26"/>
     </row>
-    <row r="22" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:21" x14ac:dyDescent="0.2">
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
       <c r="R22" s="26"/>
@@ -4985,7 +5009,13 @@
       <c r="T22" s="26"/>
       <c r="U22" s="26"/>
     </row>
-    <row r="23" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>8650</v>
+      </c>
+      <c r="H23">
+        <v>8699</v>
+      </c>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
       <c r="R23" s="26"/>
@@ -4993,7 +5023,13 @@
       <c r="T23" s="26"/>
       <c r="U23" s="26"/>
     </row>
-    <row r="24" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>8302</v>
+      </c>
+      <c r="H24">
+        <v>8349</v>
+      </c>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
       <c r="R24" s="26"/>
@@ -5001,7 +5037,13 @@
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
     </row>
-    <row r="25" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>3000</v>
+      </c>
+      <c r="H25">
+        <v>3099</v>
+      </c>
       <c r="P25" s="26"/>
       <c r="Q25" s="26"/>
       <c r="R25" s="26"/>
@@ -5009,7 +5051,13 @@
       <c r="T25" s="26"/>
       <c r="U25" s="26"/>
     </row>
-    <row r="26" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>8750</v>
+      </c>
+      <c r="H26">
+        <v>8799</v>
+      </c>
       <c r="P26" s="26"/>
       <c r="Q26" s="26"/>
       <c r="R26" s="26"/>
@@ -5017,7 +5065,7 @@
       <c r="T26" s="26"/>
       <c r="U26" s="26"/>
     </row>
-    <row r="27" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:21" x14ac:dyDescent="0.2">
       <c r="P27" s="26"/>
       <c r="Q27" s="26"/>
       <c r="R27" s="26"/>
@@ -5025,7 +5073,7 @@
       <c r="T27" s="26"/>
       <c r="U27" s="26"/>
     </row>
-    <row r="28" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:21" x14ac:dyDescent="0.2">
       <c r="P28" s="26"/>
       <c r="Q28" s="26"/>
       <c r="R28" s="26"/>
@@ -5033,7 +5081,7 @@
       <c r="T28" s="26"/>
       <c r="U28" s="26"/>
     </row>
-    <row r="29" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:21" x14ac:dyDescent="0.2">
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
       <c r="R29" s="26"/>
@@ -5041,7 +5089,7 @@
       <c r="T29" s="26"/>
       <c r="U29" s="26"/>
     </row>
-    <row r="30" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:21" x14ac:dyDescent="0.2">
       <c r="P30" s="26"/>
       <c r="Q30" s="26"/>
       <c r="R30" s="26"/>
@@ -5049,7 +5097,7 @@
       <c r="T30" s="26"/>
       <c r="U30" s="26"/>
     </row>
-    <row r="31" spans="16:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:21" x14ac:dyDescent="0.2">
       <c r="P31" s="26"/>
       <c r="Q31" s="26"/>
       <c r="R31" s="26"/>
@@ -5085,48 +5133,48 @@
   </sheetPr>
   <dimension ref="A2:AK37"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="E4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H27" sqref="H27:H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.90625" customWidth="1"/>
-    <col min="12" max="12" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1796875" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.6328125" customWidth="1"/>
-    <col min="17" max="17" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.453125" customWidth="1"/>
-    <col min="35" max="35" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="2.26953125" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.5703125" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.42578125" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="2.28515625" customWidth="1"/>
     <col min="37" max="37" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -5143,7 +5191,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -5160,7 +5208,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -5177,7 +5225,7 @@
         <v>8330</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>88</v>
       </c>
@@ -5194,7 +5242,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>90</v>
       </c>
@@ -5211,12 +5259,12 @@
         <v>590</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="AK8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -5326,7 +5374,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -5436,7 +5484,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -5546,12 +5594,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>573</v>
       </c>
@@ -5559,12 +5607,12 @@
         <v>574</v>
       </c>
     </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:8" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>578</v>
       </c>
@@ -5575,47 +5623,47 @@
         <v>577</v>
       </c>
     </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:8" x14ac:dyDescent="0.2">
       <c r="F22" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:8" x14ac:dyDescent="0.2">
       <c r="F23" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:8" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:8" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:8" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H34">
         <v>8750</v>
       </c>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H35">
         <v>8300</v>
       </c>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H36">
         <v>8650</v>
       </c>
     </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H37">
         <v>3000</v>
       </c>
@@ -5647,33 +5695,33 @@
   <dimension ref="A2:V27"/>
   <sheetViews>
     <sheetView topLeftCell="F15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19:O27"/>
+      <selection activeCell="O25" sqref="O25:O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.08984375" customWidth="1"/>
-    <col min="21" max="21" width="8.7265625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.140625" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -5690,7 +5738,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -5707,7 +5755,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>88</v>
       </c>
@@ -5724,7 +5772,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>90</v>
       </c>
@@ -5741,12 +5789,12 @@
         <v>603</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="V7" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -5808,7 +5856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -5870,7 +5918,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -5932,47 +5980,47 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O19">
         <v>8650</v>
       </c>
     </row>
-    <row r="20" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O20">
         <v>8750</v>
       </c>
     </row>
-    <row r="21" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O21">
         <v>3000</v>
       </c>
     </row>
-    <row r="22" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O22">
         <v>8300</v>
       </c>
     </row>
-    <row r="23" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O23" s="16" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="24" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O24" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="25" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O25" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="26" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O26" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="27" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="15:15" x14ac:dyDescent="0.2">
       <c r="O27" t="s">
         <v>593</v>
       </c>
@@ -6001,44 +6049,44 @@
   </sheetPr>
   <dimension ref="A2:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.1796875" customWidth="1"/>
-    <col min="15" max="15" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
-    <col min="22" max="22" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>83</v>
       </c>
@@ -6055,7 +6103,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>82</v>
       </c>
@@ -6072,7 +6120,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>239</v>
       </c>
@@ -6089,7 +6137,7 @@
         <v>5221</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -6106,7 +6154,7 @@
         <v>8330</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>88</v>
       </c>
@@ -6123,7 +6171,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>90</v>
       </c>
@@ -6140,7 +6188,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>238</v>
       </c>
@@ -6157,7 +6205,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>235</v>
       </c>
@@ -6174,12 +6222,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="AF11" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
@@ -6274,7 +6322,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -6369,7 +6417,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -6464,115 +6512,115 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="20" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N20" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="21" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N21" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="22" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N22" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="24" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N24" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="26" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N26" s="8" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="27" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N27" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="30" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N30" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N31" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N36">
         <v>5241</v>
       </c>
     </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N37">
         <v>5211</v>
       </c>
     </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N38">
         <v>5251</v>
       </c>
     </row>
-    <row r="39" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N39">
         <v>5221</v>
       </c>
     </row>
-    <row r="40" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N40" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="42" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N42">
         <v>8650</v>
       </c>
     </row>
-    <row r="43" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N43">
         <v>8750</v>
       </c>
     </row>
-    <row r="44" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N44">
         <v>3000</v>
       </c>
     </row>
-    <row r="45" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N45">
         <v>8330</v>
       </c>
     </row>
-    <row r="46" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N46" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N47" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="48" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N48" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N49" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N50" t="s">
         <v>595</v>
       </c>
@@ -6603,13 +6651,13 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.08984375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
@@ -6617,7 +6665,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="5">
         <v>5</v>
       </c>
@@ -6625,7 +6673,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="5">
         <v>10</v>
       </c>
@@ -6633,7 +6681,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>20</v>
       </c>
@@ -6641,7 +6689,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>30</v>
       </c>
@@ -6649,7 +6697,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>244</v>
       </c>
@@ -6657,7 +6705,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>40</v>
       </c>
@@ -6665,7 +6713,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>41</v>
       </c>
@@ -6673,7 +6721,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
         <v>43</v>
       </c>
@@ -6681,7 +6729,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
         <v>44</v>
       </c>
@@ -6689,7 +6737,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
         <v>46</v>
       </c>
@@ -6697,7 +6745,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
         <v>48</v>
       </c>
@@ -6705,7 +6753,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>49</v>
       </c>
@@ -6713,7 +6761,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>253</v>
       </c>
@@ -6721,7 +6769,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>255</v>
       </c>
@@ -6729,7 +6777,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>257</v>
       </c>
@@ -6737,7 +6785,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>259</v>
       </c>
@@ -6745,7 +6793,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>261</v>
       </c>
@@ -6753,7 +6801,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>263</v>
       </c>
@@ -6761,7 +6809,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>265</v>
       </c>
@@ -6769,7 +6817,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>267</v>
       </c>
@@ -6777,7 +6825,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="5">
         <v>50</v>
       </c>
@@ -6785,7 +6833,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="5">
         <v>52</v>
       </c>
@@ -6793,7 +6841,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="5">
         <v>60</v>
       </c>
@@ -6801,7 +6849,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="5">
         <v>70</v>
       </c>
@@ -6809,7 +6857,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="5">
         <v>80</v>
       </c>
@@ -6817,7 +6865,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="5">
         <v>90</v>
       </c>
@@ -6825,7 +6873,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>275</v>
       </c>
@@ -6833,7 +6881,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>277</v>
       </c>
@@ -6841,7 +6889,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>279</v>
       </c>
@@ -6849,7 +6897,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
         <v>281</v>
       </c>
@@ -6857,7 +6905,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>283</v>
       </c>
@@ -6865,7 +6913,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>285</v>
       </c>
@@ -6873,7 +6921,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>287</v>
       </c>
@@ -6881,7 +6929,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>289</v>
       </c>
@@ -6889,7 +6937,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>291</v>
       </c>
@@ -6897,7 +6945,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>293</v>
       </c>
@@ -6905,7 +6953,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>295</v>
       </c>
@@ -6913,7 +6961,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>297</v>
       </c>
@@ -6921,7 +6969,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
         <v>299</v>
       </c>
@@ -6929,7 +6977,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>301</v>
       </c>
@@ -6937,7 +6985,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
         <v>303</v>
       </c>
@@ -6945,7 +6993,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>305</v>
       </c>
@@ -6953,7 +7001,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>307</v>
       </c>
@@ -6961,7 +7009,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="5" t="s">
         <v>309</v>
       </c>
@@ -6969,7 +7017,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="5" t="s">
         <v>311</v>
       </c>
@@ -6996,13 +7044,13 @@
       <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>1</v>
       </c>
@@ -7010,7 +7058,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3">
         <v>2</v>
       </c>
@@ -7018,7 +7066,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>3</v>
       </c>
@@ -7026,7 +7074,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>4</v>
       </c>
@@ -7034,7 +7082,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6">
         <v>5</v>
       </c>
@@ -7042,7 +7090,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>6</v>
       </c>
@@ -7050,7 +7098,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>7</v>
       </c>
@@ -7058,7 +7106,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>8</v>
       </c>
@@ -7066,7 +7114,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>9</v>
       </c>
@@ -7074,7 +7122,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>10</v>
       </c>
@@ -7082,7 +7130,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>11</v>
       </c>
@@ -7090,7 +7138,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>12</v>
       </c>
@@ -7098,7 +7146,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>13</v>
       </c>
@@ -7106,7 +7154,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>14</v>
       </c>
@@ -7114,7 +7162,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>15</v>
       </c>
@@ -7122,7 +7170,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>16</v>
       </c>
@@ -7130,7 +7178,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>17</v>
       </c>
@@ -7138,7 +7186,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>18</v>
       </c>
@@ -7146,7 +7194,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>19</v>
       </c>
@@ -7154,7 +7202,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>20</v>
       </c>
@@ -7162,7 +7210,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22">
         <v>22</v>
       </c>
@@ -7170,7 +7218,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>23</v>
       </c>
@@ -7178,7 +7226,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>24</v>
       </c>
@@ -7186,7 +7234,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25">
         <v>25</v>
       </c>
@@ -7194,7 +7242,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26">
         <v>26</v>
       </c>
@@ -7202,7 +7250,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>27</v>
       </c>
@@ -7210,7 +7258,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28">
         <v>29</v>
       </c>
@@ -7218,7 +7266,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C29">
         <v>30</v>
       </c>
@@ -7226,7 +7274,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30">
         <v>45</v>
       </c>
@@ -7234,7 +7282,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C31">
         <v>71</v>
       </c>
@@ -7242,7 +7290,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C32">
         <v>72</v>
       </c>
@@ -7250,7 +7298,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33">
         <v>77</v>
       </c>
@@ -7258,7 +7306,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C34">
         <v>89</v>
       </c>
@@ -7266,7 +7314,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C35">
         <v>91</v>
       </c>
@@ -7274,7 +7322,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36">
         <v>92</v>
       </c>
@@ -7282,7 +7330,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C37">
         <v>93</v>
       </c>
@@ -7290,7 +7338,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C38">
         <v>94</v>
       </c>
@@ -7298,7 +7346,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C39">
         <v>96</v>
       </c>
@@ -7306,7 +7354,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C40">
         <v>109</v>
       </c>
@@ -7314,7 +7362,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C41">
         <v>197</v>
       </c>
@@ -7322,7 +7370,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C42">
         <v>227</v>
       </c>
@@ -7330,7 +7378,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C43">
         <v>306</v>
       </c>
@@ -7338,7 +7386,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C44">
         <v>438</v>
       </c>
@@ -7346,7 +7394,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C45">
         <v>486</v>
       </c>
@@ -7354,7 +7402,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C46">
         <v>529</v>
       </c>
@@ -7362,7 +7410,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C47">
         <v>532</v>
       </c>
@@ -7370,7 +7418,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C48">
         <v>578</v>
       </c>
@@ -7378,7 +7426,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C49">
         <v>592</v>
       </c>
@@ -7386,7 +7434,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C50">
         <v>597</v>
       </c>
@@ -7394,7 +7442,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C51">
         <v>604</v>
       </c>
@@ -7402,7 +7450,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C52">
         <v>606</v>
       </c>
@@ -7410,7 +7458,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C53">
         <v>625</v>
       </c>
@@ -7418,7 +7466,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C54">
         <v>676</v>
       </c>
@@ -7426,7 +7474,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C55">
         <v>808</v>
       </c>
@@ -7434,7 +7482,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C56">
         <v>821</v>
       </c>
@@ -7442,7 +7490,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C57">
         <v>823</v>
       </c>
@@ -7450,7 +7498,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C58">
         <v>824</v>
       </c>
@@ -7458,7 +7506,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C59">
         <v>839</v>
       </c>
@@ -7466,7 +7514,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C60">
         <v>840</v>
       </c>
@@ -7474,7 +7522,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C61">
         <v>843</v>
       </c>
@@ -7482,7 +7530,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C62">
         <v>851</v>
       </c>
@@ -7490,7 +7538,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C63">
         <v>859</v>
       </c>
@@ -7498,7 +7546,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C64">
         <v>929</v>
       </c>
@@ -7506,7 +7554,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>376</v>
       </c>
@@ -7514,7 +7562,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>378</v>
       </c>
@@ -7522,7 +7570,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>379</v>
       </c>
@@ -7530,7 +7578,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
         <v>380</v>
       </c>
@@ -7538,7 +7586,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>381</v>
       </c>
@@ -7546,7 +7594,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
         <v>383</v>
       </c>
@@ -7554,7 +7602,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
         <v>385</v>
       </c>
@@ -7562,7 +7610,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
         <v>387</v>
       </c>
@@ -7570,7 +7618,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
         <v>389</v>
       </c>
@@ -7578,7 +7626,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>391</v>
       </c>
@@ -7586,7 +7634,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>393</v>
       </c>
@@ -7594,7 +7642,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
         <v>395</v>
       </c>
@@ -7602,7 +7650,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
         <v>397</v>
       </c>
@@ -7610,7 +7658,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
         <v>399</v>
       </c>
@@ -7618,7 +7666,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
         <v>401</v>
       </c>
@@ -7626,7 +7674,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>403</v>
       </c>
@@ -7634,7 +7682,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
         <v>404</v>
       </c>
@@ -7642,7 +7690,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
         <v>405</v>
       </c>
@@ -7650,7 +7698,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
         <v>407</v>
       </c>
@@ -7658,7 +7706,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>409</v>
       </c>
@@ -7666,7 +7714,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
         <v>411</v>
       </c>
@@ -7674,7 +7722,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
         <v>413</v>
       </c>
@@ -7682,7 +7730,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
         <v>415</v>
       </c>
@@ -7690,7 +7738,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
         <v>417</v>
       </c>
@@ -7698,7 +7746,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
         <v>419</v>
       </c>
@@ -7706,7 +7754,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
         <v>421</v>
       </c>
@@ -7714,7 +7762,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
         <v>423</v>
       </c>
@@ -7722,7 +7770,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
         <v>424</v>
       </c>
@@ -7730,7 +7778,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
         <v>425</v>
       </c>
@@ -7738,7 +7786,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
         <v>427</v>
       </c>
@@ -7746,7 +7794,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
         <v>428</v>
       </c>
@@ -7754,7 +7802,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C96" t="s">
         <v>430</v>
       </c>
@@ -7762,7 +7810,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
         <v>431</v>
       </c>
@@ -7770,7 +7818,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C98" t="s">
         <v>433</v>
       </c>
@@ -7778,7 +7826,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>434</v>
       </c>
@@ -7786,7 +7834,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C100" t="s">
         <v>435</v>
       </c>
@@ -7794,7 +7842,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
         <v>436</v>
       </c>
@@ -7802,7 +7850,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
         <v>437</v>
       </c>
@@ -7810,7 +7858,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
         <v>438</v>
       </c>
@@ -7818,7 +7866,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
         <v>439</v>
       </c>
@@ -7826,7 +7874,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
         <v>440</v>
       </c>
@@ -7834,7 +7882,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C106" t="s">
         <v>442</v>
       </c>
@@ -7842,7 +7890,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
         <v>444</v>
       </c>
@@ -7850,7 +7898,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
         <v>446</v>
       </c>
@@ -7874,15 +7922,15 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>454</v>
       </c>
@@ -7902,7 +7950,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>448</v>
       </c>
@@ -7920,7 +7968,7 @@
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>449</v>
       </c>
@@ -7939,7 +7987,7 @@
       <c r="G3" s="9"/>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>450</v>
       </c>
@@ -7960,7 +8008,7 @@
         <v>8650</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>450</v>
       </c>
@@ -7981,7 +8029,7 @@
         <v>8663</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>450</v>
       </c>
@@ -8002,7 +8050,7 @@
         <v>8655</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>450</v>
       </c>
@@ -8023,7 +8071,7 @@
         <v>8658</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>450</v>
       </c>
@@ -8044,7 +8092,7 @@
         <v>8662</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>451</v>
       </c>
@@ -8065,7 +8113,7 @@
         <v>8750</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>452</v>
       </c>
@@ -8088,7 +8136,7 @@
         <v>8760</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
         <v>562</v>
@@ -8105,7 +8153,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>572</v>
       </c>
@@ -8120,17 +8168,17 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K13" s="13">
         <v>3010</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K14" s="14">
         <v>3014</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="F15" t="s">
         <v>119</v>
       </c>
@@ -8141,7 +8189,7 @@
         <v>3016</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="F16">
         <v>8750</v>
       </c>
@@ -8152,7 +8200,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F17">
         <v>8750</v>
       </c>
@@ -8163,7 +8211,7 @@
         <v>3022</v>
       </c>
     </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F18">
         <v>8300</v>
       </c>
@@ -8174,7 +8222,7 @@
         <v>8330</v>
       </c>
     </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F19">
         <v>8300</v>
       </c>
@@ -8182,7 +8230,7 @@
         <v>8302</v>
       </c>
     </row>
-    <row r="20" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F20">
         <v>8650</v>
       </c>
@@ -8190,7 +8238,7 @@
         <v>8650</v>
       </c>
     </row>
-    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F21">
         <v>8650</v>
       </c>
@@ -8201,7 +8249,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F22">
         <v>8650</v>
       </c>
@@ -8212,7 +8260,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="23" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F23">
         <v>8650</v>
       </c>
@@ -8220,7 +8268,7 @@
         <v>8658</v>
       </c>
     </row>
-    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F24">
         <v>8650</v>
       </c>
@@ -8231,7 +8279,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="25" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F25">
         <v>8650</v>
       </c>
@@ -8239,7 +8287,7 @@
         <v>8651</v>
       </c>
     </row>
-    <row r="26" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F26">
         <v>3000</v>
       </c>
@@ -8247,7 +8295,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="27" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F27">
         <v>3000</v>
       </c>
@@ -8255,7 +8303,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="28" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F28">
         <v>3000</v>
       </c>
@@ -8263,7 +8311,7 @@
         <v>3010</v>
       </c>
     </row>
-    <row r="29" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F29">
         <v>3000</v>
       </c>
@@ -8271,7 +8319,7 @@
         <v>3014</v>
       </c>
     </row>
-    <row r="30" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F30">
         <v>3000</v>
       </c>
@@ -8279,7 +8327,7 @@
         <v>3016</v>
       </c>
     </row>
-    <row r="31" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F31">
         <v>3000</v>
       </c>
@@ -8287,7 +8335,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="32" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F32">
         <v>3000</v>
       </c>
@@ -8295,7 +8343,7 @@
         <v>3022</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39">
         <v>3000</v>
       </c>
@@ -8323,9 +8371,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>24</v>
       </c>
@@ -8333,7 +8381,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="2" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D2">
         <v>5</v>
       </c>
@@ -8341,7 +8389,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D3">
         <v>10</v>
       </c>
@@ -8349,7 +8397,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D4">
         <v>20</v>
       </c>
@@ -8357,7 +8405,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D5">
         <v>30</v>
       </c>
@@ -8365,7 +8413,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>244</v>
       </c>
@@ -8373,7 +8421,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D7">
         <v>40</v>
       </c>
@@ -8381,7 +8429,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>41</v>
       </c>
@@ -8389,7 +8437,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>43</v>
       </c>
@@ -8397,7 +8445,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>44</v>
       </c>
@@ -8405,7 +8453,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>46</v>
       </c>
@@ -8413,7 +8461,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>48</v>
       </c>
@@ -8421,7 +8469,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>49</v>
       </c>
@@ -8429,7 +8477,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>253</v>
       </c>
@@ -8437,7 +8485,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>255</v>
       </c>
@@ -8445,7 +8493,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>257</v>
       </c>
@@ -8453,7 +8501,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>259</v>
       </c>
@@ -8461,7 +8509,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>261</v>
       </c>
@@ -8469,7 +8517,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>263</v>
       </c>
@@ -8477,7 +8525,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>265</v>
       </c>
@@ -8485,7 +8533,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>267</v>
       </c>
@@ -8493,7 +8541,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22">
         <v>50</v>
       </c>
@@ -8501,7 +8549,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23">
         <v>52</v>
       </c>
@@ -8509,7 +8557,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24">
         <v>60</v>
       </c>
@@ -8517,7 +8565,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25">
         <v>70</v>
       </c>
@@ -8525,7 +8573,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26">
         <v>80</v>
       </c>
@@ -8533,7 +8581,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27">
         <v>90</v>
       </c>
@@ -8541,7 +8589,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>275</v>
       </c>
@@ -8549,7 +8597,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>277</v>
       </c>
@@ -8557,7 +8605,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>279</v>
       </c>
@@ -8565,7 +8613,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>281</v>
       </c>
@@ -8573,7 +8621,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
         <v>283</v>
       </c>
@@ -8581,7 +8629,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>285</v>
       </c>
@@ -8589,7 +8637,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>287</v>
       </c>
@@ -8597,7 +8645,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>289</v>
       </c>
@@ -8605,7 +8653,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>291</v>
       </c>
@@ -8613,7 +8661,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>293</v>
       </c>
@@ -8621,7 +8669,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
         <v>295</v>
       </c>
@@ -8629,7 +8677,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
         <v>297</v>
       </c>
@@ -8637,7 +8685,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>299</v>
       </c>
@@ -8645,7 +8693,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
         <v>301</v>
       </c>
@@ -8653,7 +8701,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>303</v>
       </c>
@@ -8661,7 +8709,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
         <v>305</v>
       </c>
@@ -8669,7 +8717,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
         <v>307</v>
       </c>
@@ -8677,7 +8725,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
         <v>309</v>
       </c>
@@ -8685,7 +8733,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
         <v>311</v>
       </c>

</xml_diff>